<commit_message>
Update Build (View Changes in Describe)
Add Audio System (Fade In, Fade Out, Clip & PlayableAsset, Reduce while dialogue)
Add Audio Clip (Bgm)
Add Ending Table(Scriptable Sripte)
Add Tendency Table(Scriptable Sripte)
Add ObjectPoolHelper

Update Save System (Save Only Active Scene -> Save All Scene Data)
Update Player System (여러 인터랙션이 겹쳐 있어도 가까운 것으로 작동)
Update ShadowGame - Tutorial

Fix Inventory(necklace) - Text Color
Fix AudioSlider - Toggle
Fix SceneLoader - Fade Error (Time.unscaledDeltaTime(Dynamic) -> Fixed Time)
Fix Dialogue System - CutScene Skip
Fix - CampingGame - On Change Map(Fade), Item Color Alpha(did not change) Error
Fix - SnowMountain - Sign MiniGame Error (Text Error)
Fix - Interaction Key(Keyboard key Floating UI) divide (Tutorial, Interaction Key)

Remove not used assets
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Ending.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Ending.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64937CD-BA34-4276-9946-15337018583C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E804356-2B7B-4AB0-AA62-60B4A6FA8F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="151">
   <si>
     <t>파일명</t>
   </si>
@@ -939,9 +939,6 @@
   </si>
   <si>
     <t>(컷 씬)&gt; (스테이지 필드)</t>
-  </si>
-  <si>
-    <t>Hold, Reset</t>
   </si>
   <si>
     <t>···제 가족은 모두 죽은 건가요?</t>
@@ -1219,10 +1216,6 @@
   </si>
   <si>
     <t>···그래도 할 수만 있다면 여전히 그들과 다시금 행복하고 싶어.</t>
-  </si>
-  <si>
-    <t>Hold, -1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>Reset</t>
@@ -1290,6 +1283,18 @@
       </rPr>
       <t>인내</t>
     </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left, Appear</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Left, InActive</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hold, -1, Reset</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -2706,7 +2711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3861,9 +3868,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -3950,6 +3959,12 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="2" t="s">
@@ -3983,63 +3998,75 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
+      <c r="F8" s="7" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>6</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="15" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="16" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
@@ -5026,6 +5053,7 @@
     <row r="998" ht="16.5" customHeight="1"/>
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
+    <row r="1001" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -5038,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5146,8 +5174,8 @@
       <c r="C7" s="1">
         <v>6</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>51</v>
+      <c r="F7" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1">
@@ -5155,24 +5183,20 @@
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -5183,7 +5207,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -5194,7 +5218,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -5202,24 +5226,24 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1">
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2">
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
@@ -5227,7 +5251,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -5235,10 +5259,10 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -5246,10 +5270,10 @@
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -5257,10 +5281,10 @@
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -5271,7 +5295,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -5282,7 +5306,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -5293,7 +5317,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -5304,7 +5328,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -5312,10 +5336,10 @@
     </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -5326,7 +5350,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -5334,35 +5358,35 @@
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="1">
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" customHeight="1">
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1">
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" customHeight="1">
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1">
         <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" customHeight="1">
@@ -5370,7 +5394,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -5378,10 +5402,10 @@
     </row>
     <row r="28" spans="1:6" ht="16.5" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -5392,7 +5416,7 @@
         <v>21</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -5400,10 +5424,10 @@
     </row>
     <row r="30" spans="1:6" ht="16.5" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -5411,46 +5435,46 @@
     </row>
     <row r="31" spans="1:6" ht="16.5" customHeight="1">
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1">
         <v>6</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="16.5" customHeight="1">
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1">
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16.5" customHeight="1">
       <c r="B33" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1">
         <v>6</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16.5" customHeight="1">
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1">
         <v>6</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="16.5" customHeight="1">
@@ -5458,7 +5482,7 @@
         <v>21</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
@@ -5466,10 +5490,10 @@
     </row>
     <row r="36" spans="1:6" ht="16.5" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
@@ -5477,10 +5501,10 @@
     </row>
     <row r="37" spans="1:6" ht="16.5" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
@@ -5491,7 +5515,7 @@
         <v>21</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
@@ -5499,21 +5523,21 @@
     </row>
     <row r="39" spans="1:6" ht="16.5" customHeight="1">
       <c r="B39" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1">
         <v>6</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16.5" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
@@ -5524,7 +5548,7 @@
         <v>21</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -5532,13 +5556,13 @@
     </row>
     <row r="42" spans="1:6" ht="16.5" customHeight="1">
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1">
         <v>6</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="16.5" customHeight="1">
@@ -5546,7 +5570,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
@@ -5554,13 +5578,13 @@
     </row>
     <row r="44" spans="1:6" ht="16.5" customHeight="1">
       <c r="B44" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1">
         <v>6</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="16.5" customHeight="1">
@@ -5568,7 +5592,7 @@
         <v>21</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
@@ -5576,13 +5600,13 @@
     </row>
     <row r="46" spans="1:6" ht="16.5" customHeight="1">
       <c r="B46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" s="1">
         <v>6</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="16.5" customHeight="1">
@@ -5590,7 +5614,7 @@
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
@@ -5598,43 +5622,43 @@
     </row>
     <row r="48" spans="1:6" ht="16.5" customHeight="1">
       <c r="B48" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C48" s="1">
         <v>6</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="16.5" customHeight="1">
       <c r="B49" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="1">
         <v>6</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5" customHeight="1">
       <c r="B50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50" s="1">
         <v>6</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="16.5" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
@@ -5645,7 +5669,7 @@
         <v>21</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -5656,7 +5680,7 @@
         <v>21</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="1">
         <v>1</v>
@@ -5664,10 +5688,10 @@
     </row>
     <row r="54" spans="1:6" ht="16.5" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="1">
         <v>1</v>
@@ -5678,7 +5702,7 @@
         <v>21</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
@@ -5689,7 +5713,7 @@
         <v>21</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
@@ -5700,7 +5724,7 @@
         <v>21</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
@@ -5708,10 +5732,10 @@
     </row>
     <row r="58" spans="1:6" ht="16.5" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
@@ -5722,7 +5746,7 @@
         <v>21</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
@@ -5730,10 +5754,10 @@
     </row>
     <row r="60" spans="1:6" ht="16.5" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
@@ -5744,7 +5768,7 @@
         <v>21</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61" s="1">
         <v>1</v>
@@ -5752,10 +5776,10 @@
     </row>
     <row r="62" spans="1:6" ht="16.5" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
@@ -5763,47 +5787,49 @@
     </row>
     <row r="63" spans="1:6" ht="16.5" customHeight="1">
       <c r="B63" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C63" s="1">
         <v>2</v>
       </c>
+      <c r="F63" s="7" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="16.5" customHeight="1">
       <c r="A64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C64" s="1">
         <v>1</v>
       </c>
-      <c r="F64" s="7" t="s">
-        <v>148</v>
-      </c>
+      <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="16.5" customHeight="1">
       <c r="B65" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" s="1">
         <v>2</v>
       </c>
+      <c r="F65" s="7" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="F66" s="7" t="s">
-        <v>149</v>
-      </c>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" ht="16.5" customHeight="1">
       <c r="C67" s="1">
@@ -5815,26 +5841,26 @@
         <v>11</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="16.5" customHeight="1">
       <c r="B69" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C69" s="1">
         <v>6</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="16.5" customHeight="1">
       <c r="A70" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C70" s="1">
         <v>1</v>
@@ -5845,7 +5871,7 @@
         <v>21</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C71" s="1">
         <v>1</v>
@@ -5853,10 +5879,10 @@
     </row>
     <row r="72" spans="1:6" ht="16.5" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
@@ -5864,21 +5890,21 @@
     </row>
     <row r="73" spans="1:6" ht="16.5" customHeight="1">
       <c r="B73" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C73" s="1">
         <v>2</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C74" s="1">
         <v>1</v>
@@ -5886,21 +5912,21 @@
     </row>
     <row r="75" spans="1:6" ht="16.5" customHeight="1">
       <c r="B75" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C75" s="1">
         <v>2</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="16.5" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C76" s="1">
         <v>1</v>
@@ -5913,24 +5939,24 @@
     </row>
     <row r="78" spans="1:6" ht="16.5" customHeight="1">
       <c r="B78" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C78" s="1">
         <v>6</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="16.5" customHeight="1">
       <c r="B79" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C79" s="1">
         <v>6</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="16.5" customHeight="1">
@@ -5938,7 +5964,7 @@
         <v>21</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C80" s="1">
         <v>1</v>
@@ -5949,7 +5975,7 @@
         <v>21</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C81" s="1">
         <v>1</v>
@@ -5957,35 +5983,35 @@
     </row>
     <row r="82" spans="1:6" ht="16.5" customHeight="1">
       <c r="B82" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C82" s="1">
         <v>6</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="16.5" customHeight="1">
       <c r="B83" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C83" s="1">
         <v>6</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="16.5" customHeight="1">
       <c r="B84" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C84" s="1">
         <v>6</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="16.5" customHeight="1">
@@ -5996,7 +6022,7 @@
         <v>6</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="16.5" customHeight="1"/>
@@ -6924,10 +6950,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6942,7 +6968,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P1" s="5"/>
     </row>
@@ -7007,39 +7033,38 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>123</v>
+      <c r="B6" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>124</v>
+      <c r="B7" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -7049,26 +7074,28 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>125</v>
+      <c r="B8" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="16.5" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
-        <v>127</v>
+      <c r="B10" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -7076,20 +7103,18 @@
     </row>
     <row r="11" spans="1:16" ht="16.5" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="16.5" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1">
         <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" customHeight="1">
@@ -7097,7 +7122,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -7108,74 +7133,72 @@
         <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="16.5" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="1">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B18" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16.5" customHeight="1">
-      <c r="B18" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>144</v>
+      <c r="F18" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B19" s="7"/>
       <c r="C19" s="1">
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.5" customHeight="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A21" s="2"/>
+    </row>
     <row r="22" spans="1:6" ht="16.5" customHeight="1"/>
-    <row r="23" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1"/>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
@@ -7238,11 +7261,11 @@
     </row>
     <row r="39" spans="1:2" ht="16.5" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="2"/>
     </row>
     <row r="40" spans="1:2" ht="16.5" customHeight="1">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:2" ht="16.5" customHeight="1">
       <c r="A41" s="2"/>
@@ -7278,15 +7301,15 @@
     </row>
     <row r="49" spans="1:26" ht="16.5" customHeight="1">
       <c r="A49" s="2"/>
-      <c r="B49" s="4"/>
+      <c r="B49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="16.5" customHeight="1">
       <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
+      <c r="B50" s="4"/>
     </row>
     <row r="51" spans="1:26" ht="16.5" customHeight="1">
       <c r="A51" s="2"/>
-      <c r="B51" s="4"/>
+      <c r="B51" s="2"/>
     </row>
     <row r="52" spans="1:26" ht="16.5" customHeight="1">
       <c r="A52" s="2"/>
@@ -7294,7 +7317,7 @@
     </row>
     <row r="53" spans="1:26" ht="16.5" customHeight="1">
       <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
+      <c r="B53" s="4"/>
     </row>
     <row r="54" spans="1:26" ht="16.5" customHeight="1">
       <c r="A54" s="2"/>
@@ -7306,27 +7329,7 @@
     </row>
     <row r="56" spans="1:26" ht="16.5" customHeight="1">
       <c r="A56" s="2"/>
-      <c r="B56" s="4"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="6"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
-      <c r="S56" s="6"/>
-      <c r="T56" s="6"/>
-      <c r="U56" s="6"/>
-      <c r="V56" s="6"/>
-      <c r="W56" s="6"/>
-      <c r="X56" s="6"/>
-      <c r="Y56" s="6"/>
-      <c r="Z56" s="6"/>
+      <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="16.5" customHeight="1">
       <c r="A57" s="2"/>
@@ -7354,14 +7357,31 @@
     </row>
     <row r="58" spans="1:26" ht="16.5" customHeight="1">
       <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
+      <c r="B58" s="4"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
+      <c r="Q58" s="6"/>
+      <c r="R58" s="6"/>
+      <c r="S58" s="6"/>
+      <c r="T58" s="6"/>
+      <c r="U58" s="6"/>
+      <c r="V58" s="6"/>
+      <c r="W58" s="6"/>
+      <c r="X58" s="6"/>
+      <c r="Y58" s="6"/>
+      <c r="Z58" s="6"/>
     </row>
     <row r="59" spans="1:26" ht="16.5" customHeight="1">
       <c r="A59" s="2"/>
-      <c r="B59" s="4"/>
+      <c r="B59" s="2"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
@@ -7369,10 +7389,13 @@
     <row r="60" spans="1:26" ht="16.5" customHeight="1">
       <c r="A60" s="2"/>
       <c r="B60" s="4"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:26" ht="16.5" customHeight="1">
       <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
+      <c r="B61" s="4"/>
     </row>
     <row r="62" spans="1:26" ht="16.5" customHeight="1">
       <c r="A62" s="2"/>
@@ -7386,134 +7409,134 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:3" ht="16.5" customHeight="1">
+    <row r="65" spans="1:2" ht="16.5" customHeight="1">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:3" ht="16.5" customHeight="1">
+    <row r="66" spans="1:2" ht="16.5" customHeight="1">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:3" ht="16.5" customHeight="1">
+    <row r="67" spans="1:2" ht="16.5" customHeight="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:3" ht="16.5" customHeight="1">
+    <row r="68" spans="1:2" ht="16.5" customHeight="1">
       <c r="A68" s="2"/>
-      <c r="B68" s="4"/>
-    </row>
-    <row r="69" spans="1:3" ht="16.5" customHeight="1">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:2" ht="16.5" customHeight="1">
       <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:3" ht="16.5" customHeight="1">
+      <c r="B69" s="4"/>
+    </row>
+    <row r="70" spans="1:2" ht="16.5" customHeight="1">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:3" ht="16.5" customHeight="1">
+    <row r="71" spans="1:2" ht="16.5" customHeight="1">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:3" ht="16.5" customHeight="1">
+    <row r="72" spans="1:2" ht="16.5" customHeight="1">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:3" ht="16.5" customHeight="1">
+    <row r="73" spans="1:2" ht="16.5" customHeight="1">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:3" ht="16.5" customHeight="1">
+    <row r="74" spans="1:2" ht="16.5" customHeight="1">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:3" ht="16.5" customHeight="1">
+    <row r="75" spans="1:2" ht="16.5" customHeight="1">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:3" ht="16.5" customHeight="1">
+    <row r="76" spans="1:2" ht="16.5" customHeight="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A77" s="3"/>
+    <row r="77" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A78" s="2"/>
+    <row r="78" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A78" s="3"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A79" s="3"/>
+    <row r="79" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:3" ht="16.5" customHeight="1">
+    <row r="80" spans="1:2" ht="16.5" customHeight="1">
       <c r="A80" s="3"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:2" ht="16.5" customHeight="1">
-      <c r="A81" s="2"/>
+    </row>
+    <row r="81" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A81" s="3"/>
       <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="1:2" ht="16.5" customHeight="1">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" ht="16.5" customHeight="1">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" ht="16.5" customHeight="1">
+    <row r="83" spans="1:3" ht="16.5" customHeight="1">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="1:2" ht="16.5" customHeight="1">
+    <row r="84" spans="1:3" ht="16.5" customHeight="1">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="1:2" ht="16.5" customHeight="1">
+    <row r="85" spans="1:3" ht="16.5" customHeight="1">
       <c r="A85" s="2"/>
-      <c r="B85" s="4"/>
-    </row>
-    <row r="86" spans="1:2" ht="16.5" customHeight="1">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" ht="16.5" customHeight="1">
       <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-    </row>
-    <row r="87" spans="1:2" ht="16.5" customHeight="1">
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:3" ht="16.5" customHeight="1">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" ht="16.5" customHeight="1">
+    <row r="88" spans="1:3" ht="16.5" customHeight="1">
       <c r="A88" s="2"/>
-      <c r="B88" s="4"/>
-    </row>
-    <row r="89" spans="1:2" ht="16.5" customHeight="1">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="1:3" ht="16.5" customHeight="1">
       <c r="A89" s="2"/>
       <c r="B89" s="4"/>
     </row>
-    <row r="90" spans="1:2" ht="16.5" customHeight="1">
+    <row r="90" spans="1:3" ht="16.5" customHeight="1">
       <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-    </row>
-    <row r="91" spans="1:2" ht="16.5" customHeight="1">
+      <c r="B90" s="4"/>
+    </row>
+    <row r="91" spans="1:3" ht="16.5" customHeight="1">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" ht="16.5" customHeight="1">
+    <row r="92" spans="1:3" ht="16.5" customHeight="1">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" ht="16.5" customHeight="1">
+    <row r="93" spans="1:3" ht="16.5" customHeight="1">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:2" ht="16.5" customHeight="1">
+    <row r="94" spans="1:3" ht="16.5" customHeight="1">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" ht="16.5" customHeight="1">
+    <row r="95" spans="1:3" ht="16.5" customHeight="1">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" ht="16.5" customHeight="1">
+    <row r="96" spans="1:3" ht="16.5" customHeight="1">
       <c r="A96" s="2"/>
-      <c r="B96" s="4"/>
+      <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" ht="16.5" customHeight="1">
       <c r="A97" s="2"/>
@@ -7521,7 +7544,7 @@
     </row>
     <row r="98" spans="1:2" ht="16.5" customHeight="1">
       <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" customHeight="1">
       <c r="A99" s="2"/>
@@ -7545,11 +7568,11 @@
     </row>
     <row r="104" spans="1:2" ht="16.5" customHeight="1">
       <c r="A104" s="2"/>
-      <c r="B104" s="4"/>
+      <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:2" ht="16.5" customHeight="1">
       <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
+      <c r="B105" s="4"/>
     </row>
     <row r="106" spans="1:2" ht="16.5" customHeight="1">
       <c r="A106" s="2"/>
@@ -7557,11 +7580,11 @@
     </row>
     <row r="107" spans="1:2" ht="16.5" customHeight="1">
       <c r="A107" s="2"/>
-      <c r="B107" s="4"/>
+      <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" ht="16.5" customHeight="1">
       <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
+      <c r="B108" s="4"/>
     </row>
     <row r="109" spans="1:2" ht="16.5" customHeight="1">
       <c r="A109" s="2"/>
@@ -7569,7 +7592,7 @@
     </row>
     <row r="110" spans="1:2" ht="16.5" customHeight="1">
       <c r="A110" s="2"/>
-      <c r="B110" s="4"/>
+      <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" ht="16.5" customHeight="1">
       <c r="A111" s="2"/>
@@ -7577,7 +7600,7 @@
     </row>
     <row r="112" spans="1:2" ht="16.5" customHeight="1">
       <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
+      <c r="B112" s="4"/>
     </row>
     <row r="113" spans="1:2" ht="16.5" customHeight="1">
       <c r="A113" s="2"/>
@@ -7613,11 +7636,11 @@
     </row>
     <row r="121" spans="1:2" ht="16.5" customHeight="1">
       <c r="A121" s="2"/>
-      <c r="B121" s="4"/>
+      <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" ht="16.5" customHeight="1">
       <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
+      <c r="B122" s="4"/>
     </row>
     <row r="123" spans="1:2" ht="16.5" customHeight="1">
       <c r="A123" s="2"/>
@@ -7625,11 +7648,11 @@
     </row>
     <row r="124" spans="1:2" ht="16.5" customHeight="1">
       <c r="A124" s="2"/>
-      <c r="B124" s="4"/>
+      <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" ht="16.5" customHeight="1">
       <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
+      <c r="B125" s="4"/>
     </row>
     <row r="126" spans="1:2" ht="16.5" customHeight="1">
       <c r="A126" s="2"/>
@@ -7649,7 +7672,7 @@
     </row>
     <row r="130" spans="1:2" ht="16.5" customHeight="1">
       <c r="A130" s="2"/>
-      <c r="B130" s="4"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" ht="16.5" customHeight="1">
       <c r="A131" s="2"/>
@@ -7657,15 +7680,18 @@
     </row>
     <row r="132" spans="1:2" ht="16.5" customHeight="1">
       <c r="A132" s="2"/>
+      <c r="B132" s="4"/>
     </row>
     <row r="133" spans="1:2" ht="16.5" customHeight="1">
       <c r="A133" s="2"/>
-      <c r="B133" s="4"/>
     </row>
     <row r="134" spans="1:2" ht="16.5" customHeight="1">
       <c r="A134" s="2"/>
-    </row>
-    <row r="135" spans="1:2" ht="16.5" customHeight="1"/>
+      <c r="B134" s="4"/>
+    </row>
+    <row r="135" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A135" s="2"/>
+    </row>
     <row r="136" spans="1:2" ht="16.5" customHeight="1"/>
     <row r="137" spans="1:2" ht="16.5" customHeight="1"/>
     <row r="138" spans="1:2" ht="16.5" customHeight="1"/>
@@ -8532,6 +8558,7 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
     <row r="1001" ht="16.5" customHeight="1"/>
+    <row r="1002" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -8542,10 +8569,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G1001"/>
+  <dimension ref="A1:G1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8560,7 +8587,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -8624,39 +8651,38 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>123</v>
+      <c r="B6" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>124</v>
+      <c r="B7" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -8666,26 +8692,28 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>125</v>
+      <c r="B8" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
-        <v>127</v>
+      <c r="B10" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -8693,20 +8721,18 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="C11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1">
         <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
@@ -8714,7 +8740,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -8725,146 +8751,143 @@
         <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="1">
+    </row>
+    <row r="17" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" customHeight="1">
+      <c r="B18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16.5" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="F18" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16.5" customHeight="1">
-      <c r="B17" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="1">
+    <row r="20" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="1">
         <v>6</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C19" s="1">
-        <v>6</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C21" s="1">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" s="1">
-        <v>6</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16.5" customHeight="1">
+    <row r="24" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1">
         <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16.5" customHeight="1"/>
-    <row r="26" spans="1:7" ht="16.5" customHeight="1"/>
-    <row r="27" spans="1:7" ht="16.5" customHeight="1"/>
-    <row r="28" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="16.5" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="26" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="27" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="28" spans="1:6" ht="16.5" customHeight="1"/>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1">
       <c r="A29" s="2"/>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:7" ht="16.5" customHeight="1">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" customHeight="1">
+    <row r="31" spans="1:6" ht="16.5" customHeight="1">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="16.5" customHeight="1">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.5" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="4"/>
-      <c r="G32" s="6"/>
+      <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="16.5" customHeight="1">
       <c r="A33" s="2"/>
@@ -8873,14 +8896,12 @@
     </row>
     <row r="34" spans="1:7" ht="16.5" customHeight="1">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+      <c r="B35" s="2"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -8888,6 +8909,9 @@
     <row r="36" spans="1:7" ht="16.5" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1">
       <c r="A37" s="2"/>
@@ -8895,7 +8919,7 @@
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="B38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" customHeight="1">
       <c r="A39" s="2"/>
@@ -8915,7 +8939,7 @@
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1">
       <c r="A43" s="2"/>
-      <c r="B43" s="4"/>
+      <c r="B43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="16.5" customHeight="1">
       <c r="A44" s="2"/>
@@ -8923,7 +8947,7 @@
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="B45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1">
       <c r="A46" s="2"/>
@@ -8954,25 +8978,25 @@
       <c r="B52" s="2"/>
     </row>
     <row r="53" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A53" s="3"/>
+      <c r="A53" s="2"/>
       <c r="B53" s="2"/>
     </row>
     <row r="54" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A54" s="2"/>
+      <c r="A54" s="3"/>
       <c r="B54" s="2"/>
     </row>
     <row r="55" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A55" s="3"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:3" ht="16.5" customHeight="1">
       <c r="A56" s="3"/>
       <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
     </row>
     <row r="57" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A57" s="2"/>
+      <c r="A57" s="3"/>
       <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:3" ht="16.5" customHeight="1">
       <c r="A58" s="2"/>
@@ -8988,11 +9012,11 @@
     </row>
     <row r="61" spans="1:3" ht="16.5" customHeight="1">
       <c r="A61" s="2"/>
-      <c r="B61" s="4"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" spans="1:3" ht="16.5" customHeight="1">
       <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
+      <c r="B62" s="4"/>
     </row>
     <row r="63" spans="1:3" ht="16.5" customHeight="1">
       <c r="A63" s="2"/>
@@ -9000,7 +9024,7 @@
     </row>
     <row r="64" spans="1:3" ht="16.5" customHeight="1">
       <c r="A64" s="2"/>
-      <c r="B64" s="4"/>
+      <c r="B64" s="2"/>
     </row>
     <row r="65" spans="1:2" ht="16.5" customHeight="1">
       <c r="A65" s="2"/>
@@ -9008,7 +9032,7 @@
     </row>
     <row r="66" spans="1:2" ht="16.5" customHeight="1">
       <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
+      <c r="B66" s="4"/>
     </row>
     <row r="67" spans="1:2" ht="16.5" customHeight="1">
       <c r="A67" s="2"/>
@@ -9032,7 +9056,7 @@
     </row>
     <row r="72" spans="1:2" ht="16.5" customHeight="1">
       <c r="A72" s="2"/>
-      <c r="B72" s="4"/>
+      <c r="B72" s="2"/>
     </row>
     <row r="73" spans="1:2" ht="16.5" customHeight="1">
       <c r="A73" s="2"/>
@@ -9040,7 +9064,7 @@
     </row>
     <row r="74" spans="1:2" ht="16.5" customHeight="1">
       <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
+      <c r="B74" s="4"/>
     </row>
     <row r="75" spans="1:2" ht="16.5" customHeight="1">
       <c r="A75" s="2"/>
@@ -9064,11 +9088,11 @@
     </row>
     <row r="80" spans="1:2" ht="16.5" customHeight="1">
       <c r="A80" s="2"/>
-      <c r="B80" s="4"/>
+      <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" ht="16.5" customHeight="1">
       <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
+      <c r="B81" s="4"/>
     </row>
     <row r="82" spans="1:2" ht="16.5" customHeight="1">
       <c r="A82" s="2"/>
@@ -9076,11 +9100,11 @@
     </row>
     <row r="83" spans="1:2" ht="16.5" customHeight="1">
       <c r="A83" s="2"/>
-      <c r="B83" s="4"/>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="16.5" customHeight="1">
       <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
+      <c r="B84" s="4"/>
     </row>
     <row r="85" spans="1:2" ht="16.5" customHeight="1">
       <c r="A85" s="2"/>
@@ -9088,7 +9112,7 @@
     </row>
     <row r="86" spans="1:2" ht="16.5" customHeight="1">
       <c r="A86" s="2"/>
-      <c r="B86" s="4"/>
+      <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" ht="16.5" customHeight="1">
       <c r="A87" s="2"/>
@@ -9096,7 +9120,7 @@
     </row>
     <row r="88" spans="1:2" ht="16.5" customHeight="1">
       <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
+      <c r="B88" s="4"/>
     </row>
     <row r="89" spans="1:2" ht="16.5" customHeight="1">
       <c r="A89" s="2"/>
@@ -9132,11 +9156,11 @@
     </row>
     <row r="97" spans="1:2" ht="16.5" customHeight="1">
       <c r="A97" s="2"/>
-      <c r="B97" s="4"/>
+      <c r="B97" s="2"/>
     </row>
     <row r="98" spans="1:2" ht="16.5" customHeight="1">
       <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
+      <c r="B98" s="4"/>
     </row>
     <row r="99" spans="1:2" ht="16.5" customHeight="1">
       <c r="A99" s="2"/>
@@ -9144,11 +9168,11 @@
     </row>
     <row r="100" spans="1:2" ht="16.5" customHeight="1">
       <c r="A100" s="2"/>
-      <c r="B100" s="4"/>
+      <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" ht="16.5" customHeight="1">
       <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
+      <c r="B101" s="4"/>
     </row>
     <row r="102" spans="1:2" ht="16.5" customHeight="1">
       <c r="A102" s="2"/>
@@ -9162,7 +9186,10 @@
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:2" ht="16.5" customHeight="1"/>
+    <row r="105" spans="1:2" ht="16.5" customHeight="1">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+    </row>
     <row r="106" spans="1:2" ht="16.5" customHeight="1"/>
     <row r="107" spans="1:2" ht="16.5" customHeight="1"/>
     <row r="108" spans="1:2" ht="16.5" customHeight="1"/>
@@ -10059,6 +10086,7 @@
     <row r="999" ht="16.5" customHeight="1"/>
     <row r="1000" ht="16.5" customHeight="1"/>
     <row r="1001" ht="16.5" customHeight="1"/>
+    <row r="1002" ht="16.5" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Update For Build (Resource, Some Error)
미니게임 오류 수정
1920 x 1080 이외 해상도 시 발생하는 오류 수정
스테이지2 인벤토리 변경
컷씬 리소스 추가
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Ending.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Ending.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Project-Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165D43E4-AFD6-402B-91BD-86C503C07DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C5C620-3444-4A02-88D6-34432665745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -786,7 +786,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="154">
   <si>
     <t>파일명</t>
   </si>
@@ -1603,10 +1603,6 @@
   </si>
   <si>
     <t>Camera:Add</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ring:Add</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -7397,7 +7393,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1">
@@ -8942,7 +8938,7 @@
   <dimension ref="A1:G1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9027,7 +9023,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
@@ -9226,9 +9222,7 @@
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>153</v>
-      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" customHeight="1">
       <c r="A24" s="2"/>

</xml_diff>